<commit_message>
fixed missing ] symbol
</commit_message>
<xml_diff>
--- a/dataset/Europe.xlsx
+++ b/dataset/Europe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\CropMapping\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78535D4-B1FA-4FE8-946B-BD518D23001A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5121CD01-30BC-482C-8EE0-68B0A412138A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,109 +36,109 @@
     <t>main_type</t>
   </si>
   <si>
+    <t>maize-weat</t>
+  </si>
+  <si>
+    <t>barley-weat</t>
+  </si>
+  <si>
+    <t>sun flower</t>
+  </si>
+  <si>
+    <t>potato, kolza</t>
+  </si>
+  <si>
+    <t>suger beat, kolza, barley</t>
+  </si>
+  <si>
+    <t>dry pulses</t>
+  </si>
+  <si>
+    <t>kolza</t>
+  </si>
+  <si>
+    <t>small for local test</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>england</t>
+  </si>
+  <si>
+    <t>spain</t>
+  </si>
+  <si>
+    <t>lithuania</t>
+  </si>
+  <si>
+    <t>hungry-romania</t>
+  </si>
+  <si>
+    <t>bulgaria-romania</t>
+  </si>
+  <si>
+    <t>denmark</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>2018-08-01</t>
+  </si>
+  <si>
+    <t>2018-09-01</t>
+  </si>
+  <si>
+    <t>2018-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[[0.3036279592750457, 52.521714872690595],
+           [0.3036279592750457, 52.46506692149697],
+           [0.4924554739234832, 52.46506692149697],
+           [0.4924554739234832, 52.521714872690595]]]</t>
+  </si>
+  <si>
+    <t>[[[-0.09707574480274594, 52.29419689960738],
+           [-0.09707574480274594, 51.89598091800008],
+           [1.064728454416004, 51.89598091800008],
+           [1.064728454416004, 52.29419689960738]]]</t>
+  </si>
+  <si>
+    <t>[[[8.353814435625866, 56.130017256142345],
+           [8.353814435625866, 55.972800409471844],
+           [8.893517804766491, 55.972800409471844],
+           [8.893517804766491, 56.130017256142345]]]</t>
+  </si>
+  <si>
+    <t>[[[-5.78509864010835, 42.5303628851066],
+           [-5.78509864010835, 41.682705242512725],
+           [-3.6757236401083504, 41.682705242512725],
+           [-3.6757236401083504, 42.5303628851066]]]</t>
+  </si>
+  <si>
+    <t>[[[25.918771761913984, 44.381576609323],
+           [25.918771761913984, 43.52344855801911],
+           [28.544504183788984, 43.52344855801911],
+           [28.544504183788984, 44.381576609323]]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[[23.339739871328824, 56.3947489126311],
+           [23.339739871328824, 55.8558881337215],
+           [24.877825808828824, 55.8558881337215],
+           [24.877825808828824, 56.3947489126311]]]</t>
+  </si>
+  <si>
+    <t>[[[20.21569807645222, 47.01854554598549],
+          [20.21569807645222, 46.16926115856152],
+          [21.60546858426472, 46.16926115856152],
+          [21.60546858426472, 47.01854554598549]]]</t>
+  </si>
+  <si>
     <t>[[[1.2897224677359675, 48.38400739957012],
           [1.2897224677359675, 47.93697958008443],
           [3.2068367255484675, 47.93697958008443],
           [3.2068367255484675, 48.38400739957012]]]</t>
-  </si>
-  <si>
-    <t>[[[20.21569807645222, 47.01854554598549],
-          [20.21569807645222, 46.16926115856152],
-          [21.60546858426472, 46.16926115856152],
-          [21.60546858426472, 47.01854554598549]]]</t>
-  </si>
-  <si>
-    <t>[[[8.353814435625866, 56.130017256142345],
-           [8.353814435625866, 55.972800409471844],
-           [8.893517804766491, 55.972800409471844],
-           [8.893517804766491, 56.130017256142345]]]]</t>
-  </si>
-  <si>
-    <t>[[[-5.78509864010835, 42.5303628851066],
-           [-5.78509864010835, 41.682705242512725],
-           [-3.6757236401083504, 41.682705242512725],
-           [-3.6757236401083504, 42.5303628851066]]]]</t>
-  </si>
-  <si>
-    <t>[[[25.918771761913984, 44.381576609323],
-           [25.918771761913984, 43.52344855801911],
-           [28.544504183788984, 43.52344855801911],
-           [28.544504183788984, 44.381576609323]]]]</t>
-  </si>
-  <si>
-    <t>maize-weat</t>
-  </si>
-  <si>
-    <t>barley-weat</t>
-  </si>
-  <si>
-    <t>sun flower</t>
-  </si>
-  <si>
-    <t>potato, kolza</t>
-  </si>
-  <si>
-    <t>suger beat, kolza, barley</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [[[23.339739871328824, 56.3947489126311],
-           [23.339739871328824, 55.8558881337215],
-           [24.877825808828824, 55.8558881337215],
-           [24.877825808828824, 56.3947489126311]]]]</t>
-  </si>
-  <si>
-    <t>dry pulses</t>
-  </si>
-  <si>
-    <t>[[[-0.09707574480274594, 52.29419689960738],
-           [-0.09707574480274594, 51.89598091800008],
-           [1.064728454416004, 51.89598091800008],
-           [1.064728454416004, 52.29419689960738]]]]</t>
-  </si>
-  <si>
-    <t>kolza</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [[[0.3036279592750457, 52.521714872690595],
-           [0.3036279592750457, 52.46506692149697],
-           [0.4924554739234832, 52.46506692149697],
-           [0.4924554739234832, 52.521714872690595]]]]</t>
-  </si>
-  <si>
-    <t>small for local test</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>england</t>
-  </si>
-  <si>
-    <t>spain</t>
-  </si>
-  <si>
-    <t>lithuania</t>
-  </si>
-  <si>
-    <t>hungry-romania</t>
-  </si>
-  <si>
-    <t>bulgaria-romania</t>
-  </si>
-  <si>
-    <t>denmark</t>
-  </si>
-  <si>
-    <t>france</t>
-  </si>
-  <si>
-    <t>2018-08-01</t>
-  </si>
-  <si>
-    <t>2018-09-01</t>
-  </si>
-  <si>
-    <t>2018-06-01</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,119 +484,119 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated rois to habe a downloadable size
</commit_message>
<xml_diff>
--- a/dataset/Europe.xlsx
+++ b/dataset/Europe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\CropMapping\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5121CD01-30BC-482C-8EE0-68B0A412138A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC5829D-D379-4F68-A9C1-2DA8E5F6EAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,12 +72,6 @@
     <t>lithuania</t>
   </si>
   <si>
-    <t>hungry-romania</t>
-  </si>
-  <si>
-    <t>bulgaria-romania</t>
-  </si>
-  <si>
     <t>denmark</t>
   </si>
   <si>
@@ -99,46 +93,52 @@
            [0.4924554739234832, 52.521714872690595]]]</t>
   </si>
   <si>
-    <t>[[[-0.09707574480274594, 52.29419689960738],
-           [-0.09707574480274594, 51.89598091800008],
-           [1.064728454416004, 51.89598091800008],
-           [1.064728454416004, 52.29419689960738]]]</t>
-  </si>
-  <si>
     <t>[[[8.353814435625866, 56.130017256142345],
            [8.353814435625866, 55.972800409471844],
            [8.893517804766491, 55.972800409471844],
            [8.893517804766491, 56.130017256142345]]]</t>
   </si>
   <si>
-    <t>[[[-5.78509864010835, 42.5303628851066],
-           [-5.78509864010835, 41.682705242512725],
-           [-3.6757236401083504, 41.682705242512725],
-           [-3.6757236401083504, 42.5303628851066]]]</t>
-  </si>
-  <si>
-    <t>[[[25.918771761913984, 44.381576609323],
-           [25.918771761913984, 43.52344855801911],
-           [28.544504183788984, 43.52344855801911],
-           [28.544504183788984, 44.381576609323]]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [[[23.339739871328824, 56.3947489126311],
-           [23.339739871328824, 55.8558881337215],
-           [24.877825808828824, 55.8558881337215],
-           [24.877825808828824, 56.3947489126311]]]</t>
-  </si>
-  <si>
-    <t>[[[20.21569807645222, 47.01854554598549],
-          [20.21569807645222, 46.16926115856152],
-          [21.60546858426472, 46.16926115856152],
-          [21.60546858426472, 47.01854554598549]]]</t>
-  </si>
-  <si>
-    <t>[[[1.2897224677359675, 48.38400739957012],
-          [1.2897224677359675, 47.93697958008443],
-          [3.2068367255484675, 47.93697958008443],
-          [3.2068367255484675, 48.38400739957012]]]</t>
+    <t>[[[1.2866262035756648, 48.385430020942366],
+          [1.2866262035756648, 47.93473449186214],
+          [2.445683820763165, 47.93473449186214],
+          [2.445683820763165, 48.385430020942366]]]</t>
+  </si>
+  <si>
+    <t>hungry</t>
+  </si>
+  <si>
+    <t>[[[[20.33654768582722, 46.81969006391422],
+           [20.33654768582722, 46.36293233084845],
+           [21.50659163113972, 46.36293233084845],
+           [21.50659163113972, 46.81969006391422]]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[[23.559466433828824, 56.32475801105907],
+           [23.559466433828824, 55.94212139772337],
+           [24.740496707266324, 55.94212139772337],
+           [24.740496707266324, 56.32475801105907]]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [[[-0.09707574480274594, 52.29419689960738],
+           [-0.09707574480274594, 51.89598091800008],
+           [1.064728454416004, 51.89598091800008],
+           [1.064728454416004, 52.29419689960738]]]</t>
+  </si>
+  <si>
+    <t>[[[27.303049105663984, 44.042971343838296],
+           [27.303049105663984, 43.55928538069457],
+           [28.445627230663984, 43.55928538069457],
+           [28.445627230663984, 44.042971343838296]]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[[-5.73566016354585, 42.21381966999416],
+           [-5.73566016354585, 41.70731558747302],
+           [-4.57110938229585, 41.70731558747302],
+           [-4.57110938229585, 42.21381966999416]]]</t>
+  </si>
+  <si>
+    <t>bulgaria</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,10 +489,10 @@
     </row>
     <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -503,10 +503,10 @@
     </row>
     <row r="3" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -517,52 +517,52 @@
     </row>
     <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -573,24 +573,24 @@
     </row>
     <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
added france validation dataset roi
</commit_message>
<xml_diff>
--- a/dataset/Europe.xlsx
+++ b/dataset/Europe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\CropMapping\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE007F5-A3E8-40E0-B0B4-32633198FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855FDCEE-53A9-4585-99CF-0BFE3D61ECD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>roi</t>
   </si>
@@ -139,6 +139,15 @@
            [20.33654768582722, 46.36293233084845],
            [21.50659163113972, 46.36293233084845],
            [21.50659163113972, 46.81969006391422]]]</t>
+  </si>
+  <si>
+    <t>france_valid</t>
+  </si>
+  <si>
+    <t>[[[3.4341882784815203, 48.48852574424973],
+           [3.4341882784815203, 48.28423633983985],
+           [3.9986108859033953, 48.28423633983985],
+           [3.9986108859033953, 48.48852574424973]]]</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,6 +480,7 @@
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -517,7 +527,7 @@
     </row>
     <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -526,76 +536,90 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added englad valid dataset
</commit_message>
<xml_diff>
--- a/dataset/Europe.xlsx
+++ b/dataset/Europe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\CropMapping\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855FDCEE-53A9-4585-99CF-0BFE3D61ECD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD31617-0297-4605-8F4E-663E705D899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>roi</t>
   </si>
@@ -148,6 +148,9 @@
            [3.4341882784815203, 48.28423633983985],
            [3.9986108859033953, 48.28423633983985],
            [3.9986108859033953, 48.48852574424973]]]</t>
+  </si>
+  <si>
+    <t>england_valid</t>
   </si>
 </sst>
 </file>
@@ -471,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">

</xml_diff>